<commit_message>
Update on 20241112 BIG
</commit_message>
<xml_diff>
--- a/各地组播源汇总/海南.xlsx
+++ b/各地组播源汇总/海南.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="易视腾" sheetId="1" r:id="rId1"/>
-    <sheet name="可用IP地址" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="电信组播" sheetId="4" r:id="rId2"/>
+    <sheet name="可用IP地址" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">电信组播!$A$1:$E$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">易视腾!$A$1:$E$37</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="88">
   <si>
     <t>易视腾</t>
   </si>
@@ -124,6 +126,194 @@
   </si>
   <si>
     <t>三沙卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.119:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.1:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.14:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.2:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.122:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.3:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.124:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.4:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.121:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.11:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.80:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.82:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.83:5140</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.52:5140</t>
+  </si>
+  <si>
+    <t>白沙台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.118:5140</t>
+  </si>
+  <si>
+    <t>保亭台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.159:5140</t>
+  </si>
+  <si>
+    <t>澄迈台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.109:5140</t>
+  </si>
+  <si>
+    <t>儋州台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.107:5140</t>
+  </si>
+  <si>
+    <t>定安台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.110:5140</t>
+  </si>
+  <si>
+    <t>东方台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.111:5140</t>
+  </si>
+  <si>
+    <t>临高台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.155:5140</t>
+  </si>
+  <si>
+    <t>陵水台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.116:5140</t>
+  </si>
+  <si>
+    <t>琼海台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.106:5140</t>
+  </si>
+  <si>
+    <t>琼中台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.165:5140</t>
+  </si>
+  <si>
+    <t>昌江台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.108:5140</t>
+  </si>
+  <si>
+    <t>屯昌台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.117:5140</t>
+  </si>
+  <si>
+    <t>万宁综合</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.167:5140</t>
+  </si>
+  <si>
+    <t>文昌台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.105:5140</t>
+  </si>
+  <si>
+    <t>五指山台</t>
+  </si>
+  <si>
+    <t>/rtp/239.253.64.69:5140</t>
+  </si>
+  <si>
+    <t>海南风景欣赏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海口一台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海口二台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海口三台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电信组播</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逗号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>协议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1223,10 +1413,1036 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:E59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" t="s">
+        <v>82</v>
+      </c>
+      <c r="E58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E59"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1234,22 +2450,28 @@
     <col min="1" max="1" width="31.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1261,7 +2483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>